<commit_message>
numpy , pandas 정리 진행중
</commit_message>
<xml_diff>
--- a/ai/output/sales.xlsx
+++ b/ai/output/sales.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -616,6 +616,27 @@
         <v>599.98</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-01-05</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Phone</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" t="n">
+        <v>499.32</v>
+      </c>
+      <c r="E10" t="n">
+        <v>998.64</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>